<commit_message>
Update BonusClass from java tooling
Updated the java tooling code and added the xml file produced via export/import along with the spreadsheet

AB4-147
AB4-38
AB4-3
</commit_message>
<xml_diff>
--- a/Support/Docs/Civ4Archid.xlsx
+++ b/Support/Docs/Civ4Archid.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="GameSpeed" sheetId="1" r:id="rId1"/>
+    <sheet name="GameSpeed" r:id="rId1" sheetId="1"/>
+    <sheet name="BonusClassList" r:id="rId6" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
   <si>
     <t>Marathon</t>
   </si>
@@ -52,13 +53,71 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_MANUFACTURED</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_FUTURE</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_HIDDEN</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_SEAFOOD</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_GENERAL</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_FUEL</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_WONDER</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_RUSH</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_MODERN</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_LUXURY</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_GRAIN</t>
+  </si>
+  <si>
+    <t>BONUSCLASS_LIVESTOCK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +132,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="18"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,6 +164,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -249,97 +322,101 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="48">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="5" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="5" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="8" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="9" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="10" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="11" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="8" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="9" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="10" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="11" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="8" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="9" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="10" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="11" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -356,10 +433,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -394,7 +471,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -429,7 +506,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -523,21 +600,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -554,7 +631,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -606,15 +683,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -622,7 +699,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row ht="15.75" r="1" spans="1:28" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>6</v>
@@ -961,11 +1038,11 @@
         <v>140</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" ref="C6:C14" si="0">B6+C5</f>
+        <f ref="C6:C14" si="0" t="shared">B6+C5</f>
         <v>470</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D14" si="1">A6*B6+D5</f>
+        <f ref="D6:D14" si="1" t="shared">A6*B6+D5</f>
         <v>360000</v>
       </c>
       <c r="E6" s="8">
@@ -975,11 +1052,11 @@
         <v>150</v>
       </c>
       <c r="G6" s="9">
-        <f t="shared" ref="G6:G13" si="2">F6+G5</f>
+        <f ref="G6:G13" si="2" t="shared">F6+G5</f>
         <v>470</v>
       </c>
       <c r="H6" s="10">
-        <f t="shared" ref="H6:H13" si="3">E6*F6+H5</f>
+        <f ref="H6:H13" si="3" t="shared">E6*F6+H5</f>
         <v>538500</v>
       </c>
       <c r="I6" s="16">
@@ -989,11 +1066,11 @@
         <v>125</v>
       </c>
       <c r="K6" s="17">
-        <f t="shared" ref="K6:K14" si="4">J6+K5</f>
+        <f ref="K6:K14" si="4" t="shared">J6+K5</f>
         <v>400</v>
       </c>
       <c r="L6" s="18">
-        <f t="shared" ref="L6:L14" si="5">I6*J6 +L5</f>
+        <f ref="L6:L14" si="5" t="shared">I6*J6 +L5</f>
         <v>552000</v>
       </c>
       <c r="M6" s="8">
@@ -1003,11 +1080,11 @@
         <v>40</v>
       </c>
       <c r="O6" s="9">
-        <f t="shared" ref="O6:O13" si="6">N6+O5</f>
+        <f ref="O6:O13" si="6" t="shared">N6+O5</f>
         <v>190</v>
       </c>
       <c r="P6" s="10">
-        <f t="shared" ref="P6:P13" si="7">M6*N6+P5</f>
+        <f ref="P6:P13" si="7" t="shared">M6*N6+P5</f>
         <v>532000</v>
       </c>
       <c r="Q6" s="16">
@@ -1017,11 +1094,11 @@
         <v>75</v>
       </c>
       <c r="S6" s="17">
-        <f t="shared" ref="S6:S13" si="8">R6+S5</f>
+        <f ref="S6:S13" si="8" t="shared">R6+S5</f>
         <v>215</v>
       </c>
       <c r="T6" s="18">
-        <f t="shared" ref="T6:T13" si="9">Q6*R6+T5</f>
+        <f ref="T6:T13" si="9" t="shared">Q6*R6+T5</f>
         <v>588000</v>
       </c>
       <c r="U6" s="8">
@@ -1031,11 +1108,11 @@
         <v>50</v>
       </c>
       <c r="W6" s="9">
-        <f t="shared" ref="W6:W14" si="10">V6+W5</f>
+        <f ref="W6:W14" si="10" t="shared">V6+W5</f>
         <v>100</v>
       </c>
       <c r="X6" s="10">
-        <f t="shared" ref="X6:X14" si="11">U6*V6+X5</f>
+        <f ref="X6:X14" si="11" t="shared">U6*V6+X5</f>
         <v>552000</v>
       </c>
       <c r="Y6" s="16">
@@ -1045,11 +1122,11 @@
         <v>30</v>
       </c>
       <c r="AA6" s="17">
-        <f t="shared" ref="AA6:AA13" si="12">Z6+AA5</f>
+        <f ref="AA6:AA13" si="12" t="shared">Z6+AA5</f>
         <v>80</v>
       </c>
       <c r="AB6" s="18">
-        <f t="shared" ref="AB6:AB13" si="13">Y6*Z6+AB5</f>
+        <f ref="AB6:AB13" si="13" t="shared">Y6*Z6+AB5</f>
         <v>552000</v>
       </c>
     </row>
@@ -1061,11 +1138,11 @@
         <v>180</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>650</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>446400</v>
       </c>
       <c r="E7" s="8">
@@ -1075,11 +1152,11 @@
         <v>160</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>630</v>
       </c>
       <c r="H7" s="10">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>562500</v>
       </c>
       <c r="I7" s="16">
@@ -1089,11 +1166,11 @@
         <v>100</v>
       </c>
       <c r="K7" s="17">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>500</v>
       </c>
       <c r="L7" s="18">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>570000</v>
       </c>
       <c r="M7" s="8">
@@ -1103,11 +1180,11 @@
         <v>140</v>
       </c>
       <c r="O7" s="9">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>330</v>
       </c>
       <c r="P7" s="10">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>585200</v>
       </c>
       <c r="Q7" s="16">
@@ -1117,11 +1194,11 @@
         <v>60</v>
       </c>
       <c r="S7" s="17">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>275</v>
       </c>
       <c r="T7" s="18">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>606000</v>
       </c>
       <c r="U7" s="8">
@@ -1131,11 +1208,11 @@
         <v>50</v>
       </c>
       <c r="W7" s="9">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>150</v>
       </c>
       <c r="X7" s="10">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>588000</v>
       </c>
       <c r="Y7" s="16">
@@ -1145,11 +1222,11 @@
         <v>40</v>
       </c>
       <c r="AA7" s="17">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>120</v>
       </c>
       <c r="AB7" s="18">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>588000</v>
       </c>
     </row>
@@ -1161,11 +1238,11 @@
         <v>350</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1000</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>537400</v>
       </c>
       <c r="E8" s="8">
@@ -1175,11 +1252,11 @@
         <v>250</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>880</v>
       </c>
       <c r="H8" s="10">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>587500</v>
       </c>
       <c r="I8" s="16">
@@ -1189,11 +1266,11 @@
         <v>300</v>
       </c>
       <c r="K8" s="17">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>800</v>
       </c>
       <c r="L8" s="18">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>606000</v>
       </c>
       <c r="M8" s="8">
@@ -1203,11 +1280,11 @@
         <v>90</v>
       </c>
       <c r="O8" s="9">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>420</v>
       </c>
       <c r="P8" s="10">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>605000</v>
       </c>
       <c r="Q8" s="16">
@@ -1217,11 +1294,11 @@
         <v>25</v>
       </c>
       <c r="S8" s="17">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>300</v>
       </c>
       <c r="T8" s="18">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>612000</v>
       </c>
       <c r="U8" s="8">
@@ -1231,11 +1308,11 @@
         <v>30</v>
       </c>
       <c r="W8" s="9">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>180</v>
       </c>
       <c r="X8" s="10">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>602400</v>
       </c>
       <c r="Y8" s="16">
@@ -1245,11 +1322,11 @@
         <v>40</v>
       </c>
       <c r="AA8" s="17">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>160</v>
       </c>
       <c r="AB8" s="18">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>608000</v>
       </c>
     </row>
@@ -1261,11 +1338,11 @@
         <v>400</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1400</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>577400</v>
       </c>
       <c r="E9" s="8">
@@ -1275,11 +1352,11 @@
         <v>350</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>1230</v>
       </c>
       <c r="H9" s="10">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>605000</v>
       </c>
       <c r="I9" s="16">
@@ -1289,11 +1366,11 @@
         <v>170</v>
       </c>
       <c r="K9" s="17">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>970</v>
       </c>
       <c r="L9" s="18">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>616200</v>
       </c>
       <c r="M9" s="8">
@@ -1303,11 +1380,11 @@
         <v>40</v>
       </c>
       <c r="O9" s="9">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>460</v>
       </c>
       <c r="P9" s="10">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>611000</v>
       </c>
       <c r="Q9" s="16">
@@ -1317,11 +1394,11 @@
         <v>50</v>
       </c>
       <c r="S9" s="17">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>350</v>
       </c>
       <c r="T9" s="18">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>618000</v>
       </c>
       <c r="U9" s="8">
@@ -1331,11 +1408,11 @@
         <v>20</v>
       </c>
       <c r="W9" s="9">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>200</v>
       </c>
       <c r="X9" s="10">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>609600</v>
       </c>
       <c r="Y9" s="16">
@@ -1345,11 +1422,11 @@
         <v>50</v>
       </c>
       <c r="AA9" s="17">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>210</v>
       </c>
       <c r="AB9" s="18">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>620500</v>
       </c>
     </row>
@@ -1361,11 +1438,11 @@
         <v>450</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>1850</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>599900</v>
       </c>
       <c r="E10" s="8">
@@ -1375,11 +1452,11 @@
         <v>450</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>1680</v>
       </c>
       <c r="H10" s="10">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>614000</v>
       </c>
       <c r="I10" s="16">
@@ -1389,11 +1466,11 @@
         <v>221</v>
       </c>
       <c r="K10" s="17">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>1191</v>
       </c>
       <c r="L10" s="18">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>621504</v>
       </c>
       <c r="M10" s="8">
@@ -1403,11 +1480,11 @@
         <v>90</v>
       </c>
       <c r="O10" s="9">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>550</v>
       </c>
       <c r="P10" s="10">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>618200</v>
       </c>
       <c r="Q10" s="16">
@@ -1417,11 +1494,11 @@
         <v>60</v>
       </c>
       <c r="S10" s="17">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>410</v>
       </c>
       <c r="T10" s="18">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>621600</v>
       </c>
       <c r="U10" s="8">
@@ -1431,11 +1508,11 @@
         <v>30</v>
       </c>
       <c r="W10" s="9">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>230</v>
       </c>
       <c r="X10" s="10">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>616800</v>
       </c>
       <c r="Y10" s="16">
@@ -1445,11 +1522,11 @@
         <v>50</v>
       </c>
       <c r="AA10" s="17">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>260</v>
       </c>
       <c r="AB10" s="18">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>626500</v>
       </c>
     </row>
@@ -1461,11 +1538,11 @@
         <v>700</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>2550</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>613900</v>
       </c>
       <c r="E11" s="8">
@@ -1475,11 +1552,11 @@
         <v>475</v>
       </c>
       <c r="G11" s="9">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>2155</v>
       </c>
       <c r="H11" s="10">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>618750</v>
       </c>
       <c r="I11" s="16">
@@ -1489,11 +1566,11 @@
         <v>129</v>
       </c>
       <c r="K11" s="17">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>1320</v>
       </c>
       <c r="L11" s="18">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>623052</v>
       </c>
       <c r="M11" s="8">
@@ -1503,11 +1580,11 @@
         <v>70</v>
       </c>
       <c r="O11" s="9">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>620</v>
       </c>
       <c r="P11" s="10">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>620300</v>
       </c>
       <c r="Q11" s="16">
@@ -1517,11 +1594,11 @@
         <v>50</v>
       </c>
       <c r="S11" s="17">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>460</v>
       </c>
       <c r="T11" s="18">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>622800</v>
       </c>
       <c r="U11" s="8">
@@ -1531,11 +1608,11 @@
         <v>25</v>
       </c>
       <c r="W11" s="9">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>255</v>
       </c>
       <c r="X11" s="10">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>619800</v>
       </c>
       <c r="Y11" s="16">
@@ -1545,11 +1622,11 @@
         <v>40</v>
       </c>
       <c r="AA11" s="17">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>300</v>
       </c>
       <c r="AB11" s="18">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>628900</v>
       </c>
     </row>
@@ -1561,11 +1638,11 @@
         <v>650</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>3200</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>620400</v>
       </c>
       <c r="E12" s="8">
@@ -1575,11 +1652,11 @@
         <v>600</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>2755</v>
       </c>
       <c r="H12" s="10">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>621750</v>
       </c>
       <c r="I12" s="16">
@@ -1589,11 +1666,11 @@
         <v>180</v>
       </c>
       <c r="K12" s="17">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>1500</v>
       </c>
       <c r="L12" s="18">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>624132</v>
       </c>
       <c r="M12" s="8">
@@ -1603,11 +1680,11 @@
         <v>100</v>
       </c>
       <c r="O12" s="9">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>720</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>621500</v>
       </c>
       <c r="Q12" s="16">
@@ -1617,11 +1694,11 @@
         <v>100</v>
       </c>
       <c r="S12" s="17">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>560</v>
       </c>
       <c r="T12" s="18">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>624000</v>
       </c>
       <c r="U12" s="8">
@@ -1631,11 +1708,11 @@
         <v>40</v>
       </c>
       <c r="W12" s="9">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>295</v>
       </c>
       <c r="X12" s="10">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>622200</v>
       </c>
       <c r="Y12" s="16">
@@ -1645,11 +1722,11 @@
         <v>30</v>
       </c>
       <c r="AA12" s="17">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>330</v>
       </c>
       <c r="AB12" s="18">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>629500</v>
       </c>
     </row>
@@ -1661,11 +1738,11 @@
         <v>1000</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4200</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>621400</v>
       </c>
       <c r="E13" s="8">
@@ -1675,11 +1752,11 @@
         <v>745</v>
       </c>
       <c r="G13" s="11">
-        <f t="shared" si="2"/>
+        <f si="2" t="shared"/>
         <v>3500</v>
       </c>
       <c r="H13" s="12">
-        <f t="shared" si="3"/>
+        <f si="3" t="shared"/>
         <v>622495</v>
       </c>
       <c r="I13" s="16">
@@ -1689,11 +1766,11 @@
         <v>300</v>
       </c>
       <c r="K13" s="17">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>1800</v>
       </c>
       <c r="L13" s="18">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>625032</v>
       </c>
       <c r="M13" s="8">
@@ -1703,11 +1780,11 @@
         <v>220</v>
       </c>
       <c r="O13" s="11">
-        <f t="shared" si="6"/>
+        <f si="6" t="shared"/>
         <v>940</v>
       </c>
       <c r="P13" s="12">
-        <f t="shared" si="7"/>
+        <f si="7" t="shared"/>
         <v>622820</v>
       </c>
       <c r="Q13" s="16">
@@ -1717,11 +1794,11 @@
         <v>60</v>
       </c>
       <c r="S13" s="25">
-        <f t="shared" si="8"/>
+        <f si="8" t="shared"/>
         <v>620</v>
       </c>
       <c r="T13" s="26">
-        <f t="shared" si="9"/>
+        <f si="9" t="shared"/>
         <v>624240</v>
       </c>
       <c r="U13" s="8">
@@ -1731,11 +1808,11 @@
         <v>65</v>
       </c>
       <c r="W13" s="9">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>360</v>
       </c>
       <c r="X13" s="10">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>623760</v>
       </c>
       <c r="Y13" s="16">
@@ -1745,15 +1822,15 @@
         <v>20</v>
       </c>
       <c r="AA13" s="25">
-        <f t="shared" si="12"/>
+        <f si="12" t="shared"/>
         <v>350</v>
       </c>
       <c r="AB13" s="26">
-        <f t="shared" si="13"/>
+        <f si="13" t="shared"/>
         <v>629700</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="15.75" r="14" spans="1:28" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>5</v>
       </c>
@@ -1761,11 +1838,11 @@
         <v>600</v>
       </c>
       <c r="C14" s="6">
-        <f t="shared" si="0"/>
+        <f si="0" t="shared"/>
         <v>4800</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" si="1"/>
+        <f si="1" t="shared"/>
         <v>624400</v>
       </c>
       <c r="E14" s="13"/>
@@ -1779,11 +1856,11 @@
         <v>200</v>
       </c>
       <c r="K14" s="21">
-        <f t="shared" si="4"/>
+        <f si="4" t="shared"/>
         <v>2000</v>
       </c>
       <c r="L14" s="22">
-        <f t="shared" si="5"/>
+        <f si="5" t="shared"/>
         <v>625232</v>
       </c>
       <c r="M14" s="13"/>
@@ -1801,11 +1878,11 @@
         <v>70</v>
       </c>
       <c r="W14" s="23">
-        <f t="shared" si="10"/>
+        <f si="10" t="shared"/>
         <v>430</v>
       </c>
       <c r="X14" s="24">
-        <f t="shared" si="11"/>
+        <f si="11" t="shared"/>
         <v>624600</v>
       </c>
       <c r="Y14" s="19"/>
@@ -1823,7 +1900,131 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="360" orientation="portrait" r:id="rId1" verticalDpi="360"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="29.56640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.6796875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="46">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s" s="46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" ht="15.0" customHeight="true">
+      <c r="A2" t="s" s="47">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="15.0" customHeight="true">
+      <c r="A3" t="s" s="47">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="15.0" customHeight="true">
+      <c r="A4" t="s" s="47">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s" s="47">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" ht="15.0" customHeight="true">
+      <c r="A5" t="s" s="47">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="47">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" ht="15.0" customHeight="true">
+      <c r="A6" t="s" s="47">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" ht="15.0" customHeight="true">
+      <c r="A7" t="s" s="47">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s" s="47">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" ht="15.0" customHeight="true">
+      <c r="A8" t="s" s="47">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s" s="47">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" ht="15.0" customHeight="true">
+      <c r="A9" t="s" s="47">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s" s="47">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" ht="15.0" customHeight="true">
+      <c r="A10" t="s" s="47">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s" s="47">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" ht="15.0" customHeight="true">
+      <c r="A11" t="s" s="47">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s" s="47">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" ht="15.0" customHeight="true">
+      <c r="A12" t="s" s="47">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s" s="47">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" ht="15.0" customHeight="true">
+      <c r="A13" t="s" s="47">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s" s="47">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>